<commit_message>
Bausteinsicht hinzugefügt, einige Ignores und Literaturverzeichnis
</commit_message>
<xml_diff>
--- a/planung/projektplan_masterarbeit.xlsx
+++ b/planung/projektplan_masterarbeit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33900" windowHeight="21220"/>
+    <workbookView xWindow="1780" yWindow="760" windowWidth="33900" windowHeight="21220"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Projektschritt</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Legende Taskfarbmarkierung:</t>
+  </si>
+  <si>
+    <t>überfällig</t>
   </si>
 </sst>
 </file>
@@ -549,67 +552,7 @@
     <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1037,11 +980,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="604268328"/>
-        <c:axId val="604272296"/>
+        <c:axId val="2136038136"/>
+        <c:axId val="2136077224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="604268328"/>
+        <c:axId val="2136038136"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1076,7 +1019,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604272296"/>
+        <c:crossAx val="2136077224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1086,7 +1029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="604272296"/>
+        <c:axId val="2136077224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41590.0"/>
@@ -1133,7 +1076,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604268328"/>
+        <c:crossAx val="2136038136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="31.0"/>
@@ -1547,10 +1490,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1572,7 +1518,7 @@
       </c>
       <c r="E1" s="20">
         <f ca="1">TODAY()</f>
-        <v>41385</v>
+        <v>41474</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1625,7 +1571,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1643,7 +1589,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
@@ -1664,7 +1610,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>19</v>
@@ -1685,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>20</v>
@@ -1706,7 +1652,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G9" s="21"/>
     </row>
@@ -1725,7 +1671,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G10" s="21"/>
     </row>
@@ -1744,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G11" s="21"/>
     </row>
@@ -1763,7 +1709,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G12" s="21"/>
     </row>
@@ -1782,7 +1728,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1800,7 +1746,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1818,7 +1764,7 @@
         <v>16</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1836,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1854,7 +1800,7 @@
         <v>92</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24">
@@ -1929,24 +1875,24 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E4:E7 E9:E19">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="überfällig">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="überfällig">
       <formula>NOT(ISERROR(SEARCH("überfällig",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="in Bearbeitung">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="in Bearbeitung">
       <formula>NOT(ISERROR(SEARCH("in Bearbeitung",E4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Erledigt">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Erledigt">
       <formula>NOT(ISERROR(SEARCH("Erledigt",E4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="überfällig">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="überfällig">
       <formula>NOT(ISERROR(SEARCH("überfällig",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="in Bearbeitung">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="in Bearbeitung">
       <formula>NOT(ISERROR(SEARCH("in Bearbeitung",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Erledigt">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Erledigt">
       <formula>NOT(ISERROR(SEARCH("Erledigt",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1956,12 +1902,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="52" orientation="portrait"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>